<commit_message>
added kiana topic 1, section 1
</commit_message>
<xml_diff>
--- a/topics_times.xlsx
+++ b/topics_times.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katzd\Desktop\Rprojects\VLL\VLL_explore\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katzd\Desktop\Rprojects\VLL\VLL_dat\VLL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90757DB9-BC3D-45F7-8532-D24AAC779CF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C238AD78-A4AD-4AA4-9CA1-37F4341D7F3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{637B2B4F-6294-45AF-9604-BBD7385AEC85}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="133">
   <si>
     <t>Amy</t>
   </si>
@@ -798,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40D0323-6377-4054-9E66-62DBA9E95AB2}">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,7 +1465,7 @@
         <v>4</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>22</v>
@@ -1482,13 +1482,13 @@
         <v>4</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1499,13 +1499,13 @@
         <v>4</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1516,13 +1516,13 @@
         <v>4</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1533,13 +1533,13 @@
         <v>4</v>
       </c>
       <c r="C43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1550,13 +1550,13 @@
         <v>4</v>
       </c>
       <c r="C44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1567,13 +1567,13 @@
         <v>4</v>
       </c>
       <c r="C45">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1584,30 +1584,30 @@
         <v>4</v>
       </c>
       <c r="C46">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1618,13 +1618,13 @@
         <v>4</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1635,13 +1635,13 @@
         <v>4</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1652,13 +1652,13 @@
         <v>4</v>
       </c>
       <c r="C50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1669,13 +1669,13 @@
         <v>4</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1686,13 +1686,13 @@
         <v>4</v>
       </c>
       <c r="C52">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1703,13 +1703,13 @@
         <v>4</v>
       </c>
       <c r="C53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1720,13 +1720,13 @@
         <v>4</v>
       </c>
       <c r="C54">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1737,30 +1737,30 @@
         <v>4</v>
       </c>
       <c r="C55">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1771,13 +1771,13 @@
         <v>40</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E57" s="6">
-        <v>1.224537037037037E-2</v>
+        <v>41</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1788,13 +1788,13 @@
         <v>40</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E58" s="5">
-        <v>0.91319444444444453</v>
+        <v>94</v>
+      </c>
+      <c r="E58" s="6">
+        <v>1.224537037037037E-2</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1805,13 +1805,13 @@
         <v>40</v>
       </c>
       <c r="C59">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E59" s="5">
-        <v>0.91041666666666676</v>
+        <v>0.91319444444444453</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1822,13 +1822,13 @@
         <v>40</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E60" s="5">
-        <v>0.53402777777777777</v>
+        <v>0.91041666666666676</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1839,13 +1839,13 @@
         <v>40</v>
       </c>
       <c r="C61">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E61" s="5">
-        <v>1.1055555555555556</v>
+        <v>0.53402777777777777</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1856,13 +1856,13 @@
         <v>40</v>
       </c>
       <c r="C62">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E62" s="5">
-        <v>0.86736111111111114</v>
+        <v>1.1055555555555556</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1873,13 +1873,13 @@
         <v>40</v>
       </c>
       <c r="C63">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>42</v>
+        <v>99</v>
+      </c>
+      <c r="E63" s="5">
+        <v>0.86736111111111114</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1890,30 +1890,30 @@
         <v>40</v>
       </c>
       <c r="C64">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E64" s="5">
-        <v>0.62847222222222221</v>
+        <v>42</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B65" t="s">
         <v>40</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E65" s="5">
-        <v>0.35138888888888892</v>
+        <v>0.62847222222222221</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1924,13 +1924,13 @@
         <v>40</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E66" s="5">
-        <v>0.48680555555555555</v>
+        <v>0.35138888888888892</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1941,13 +1941,13 @@
         <v>40</v>
       </c>
       <c r="C67">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E67" s="5">
-        <v>0.52638888888888891</v>
+        <v>0.48680555555555555</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1958,13 +1958,13 @@
         <v>40</v>
       </c>
       <c r="C68">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E68" s="5">
-        <v>0.30555555555555552</v>
+        <v>0.52638888888888891</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1975,13 +1975,13 @@
         <v>40</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E69" s="5">
-        <v>0.44513888888888892</v>
+        <v>0.30555555555555552</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1992,13 +1992,13 @@
         <v>40</v>
       </c>
       <c r="C70">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E70" s="5">
-        <v>0.65694444444444444</v>
+        <v>0.44513888888888892</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2009,13 +2009,13 @@
         <v>40</v>
       </c>
       <c r="C71">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E71" s="5">
-        <v>0.625</v>
+        <v>0.65694444444444444</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2026,13 +2026,13 @@
         <v>40</v>
       </c>
       <c r="C72">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E72" s="5">
-        <v>0.27916666666666667</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2043,30 +2043,30 @@
         <v>40</v>
       </c>
       <c r="C73">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E73" s="5">
-        <v>0.48819444444444443</v>
+        <v>0.27916666666666667</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B74" t="s">
         <v>40</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E74" s="5">
-        <v>0.72152777777777777</v>
+        <v>0.48819444444444443</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2077,13 +2077,13 @@
         <v>40</v>
       </c>
       <c r="C75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E75" s="5">
-        <v>0.8222222222222223</v>
+        <v>0.72152777777777777</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2094,13 +2094,13 @@
         <v>40</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E76" s="5">
-        <v>0.98472222222222217</v>
+        <v>0.8222222222222223</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2111,13 +2111,13 @@
         <v>40</v>
       </c>
       <c r="C77">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E77" s="5">
-        <v>0.73541666666666661</v>
+        <v>0.98472222222222217</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2128,13 +2128,13 @@
         <v>40</v>
       </c>
       <c r="C78">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E78" s="5">
-        <v>0.69097222222222221</v>
+        <v>0.73541666666666661</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2145,13 +2145,13 @@
         <v>40</v>
       </c>
       <c r="C79">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>43</v>
+        <v>114</v>
+      </c>
+      <c r="E79" s="5">
+        <v>0.69097222222222221</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2162,13 +2162,13 @@
         <v>40</v>
       </c>
       <c r="C80">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E80" s="5">
-        <v>0.95347222222222217</v>
+        <v>43</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2179,13 +2179,13 @@
         <v>40</v>
       </c>
       <c r="C81">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E81" s="5">
-        <v>0.47916666666666669</v>
+        <v>0.95347222222222217</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2196,30 +2196,30 @@
         <v>40</v>
       </c>
       <c r="C82">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E82" s="5">
-        <v>0.7104166666666667</v>
+        <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B83" t="s">
         <v>40</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>44</v>
+        <v>117</v>
+      </c>
+      <c r="E83" s="5">
+        <v>0.7104166666666667</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2230,13 +2230,13 @@
         <v>40</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2247,13 +2247,13 @@
         <v>40</v>
       </c>
       <c r="C85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2264,13 +2264,13 @@
         <v>40</v>
       </c>
       <c r="C86">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2281,13 +2281,13 @@
         <v>40</v>
       </c>
       <c r="C87">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2298,13 +2298,13 @@
         <v>40</v>
       </c>
       <c r="C88">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2315,13 +2315,13 @@
         <v>40</v>
       </c>
       <c r="C89">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2332,13 +2332,13 @@
         <v>40</v>
       </c>
       <c r="C90">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2349,30 +2349,30 @@
         <v>40</v>
       </c>
       <c r="C91">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B92" t="s">
         <v>40</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2383,13 +2383,13 @@
         <v>40</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2400,13 +2400,13 @@
         <v>40</v>
       </c>
       <c r="C94">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2417,13 +2417,13 @@
         <v>40</v>
       </c>
       <c r="C95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2434,13 +2434,13 @@
         <v>40</v>
       </c>
       <c r="C96">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2451,13 +2451,13 @@
         <v>40</v>
       </c>
       <c r="C97">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2468,13 +2468,13 @@
         <v>40</v>
       </c>
       <c r="C98">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2485,13 +2485,13 @@
         <v>40</v>
       </c>
       <c r="C99">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2502,30 +2502,30 @@
         <v>40</v>
       </c>
       <c r="C100">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B101" t="s">
         <v>40</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2536,13 +2536,13 @@
         <v>40</v>
       </c>
       <c r="C102">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2553,13 +2553,13 @@
         <v>40</v>
       </c>
       <c r="C103">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2570,13 +2570,13 @@
         <v>40</v>
       </c>
       <c r="C104">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2587,13 +2587,13 @@
         <v>40</v>
       </c>
       <c r="C105">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2604,13 +2604,13 @@
         <v>40</v>
       </c>
       <c r="C106">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2621,13 +2621,13 @@
         <v>40</v>
       </c>
       <c r="C107">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2638,13 +2638,13 @@
         <v>40</v>
       </c>
       <c r="C108">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2655,30 +2655,30 @@
         <v>40</v>
       </c>
       <c r="C109">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E109" s="1">
-        <v>0.52152777777777781</v>
+        <v>67</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B110" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>69</v>
+        <v>118</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0.52152777777777781</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2689,13 +2689,13 @@
         <v>68</v>
       </c>
       <c r="C111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2706,13 +2706,13 @@
         <v>68</v>
       </c>
       <c r="C112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -2723,13 +2723,13 @@
         <v>68</v>
       </c>
       <c r="C113">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2740,13 +2740,13 @@
         <v>68</v>
       </c>
       <c r="C114">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -2757,13 +2757,13 @@
         <v>68</v>
       </c>
       <c r="C115">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -2774,13 +2774,13 @@
         <v>68</v>
       </c>
       <c r="C116">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2791,13 +2791,13 @@
         <v>68</v>
       </c>
       <c r="C117">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2808,13 +2808,13 @@
         <v>68</v>
       </c>
       <c r="C118">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2825,24 +2825,30 @@
         <v>68</v>
       </c>
       <c r="C119">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B120" t="s">
         <v>68</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,7 +2859,7 @@
         <v>68</v>
       </c>
       <c r="C121">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,7 +2870,7 @@
         <v>68</v>
       </c>
       <c r="C122">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -2875,7 +2881,7 @@
         <v>68</v>
       </c>
       <c r="C123">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -2886,7 +2892,7 @@
         <v>68</v>
       </c>
       <c r="C124">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -2897,7 +2903,7 @@
         <v>68</v>
       </c>
       <c r="C125">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -2908,7 +2914,7 @@
         <v>68</v>
       </c>
       <c r="C126">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -2919,7 +2925,7 @@
         <v>68</v>
       </c>
       <c r="C127">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -2930,7 +2936,7 @@
         <v>68</v>
       </c>
       <c r="C128">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -2941,7 +2947,7 @@
         <v>68</v>
       </c>
       <c r="C129">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -2949,6 +2955,17 @@
         <v>7</v>
       </c>
       <c r="B130" t="s">
+        <v>68</v>
+      </c>
+      <c r="C130">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>